<commit_message>
Update named ranges/tables in config.xlsx
</commit_message>
<xml_diff>
--- a/static/examples/config.xlsx
+++ b/static/examples/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YinChi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\yinchi\digital-hospitals\frontend\static\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99469912-0BA3-43F2-A24F-D651DF5EEF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B5D908-1806-4013-A41B-4B1C456F3835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="41268" windowHeight="21480" tabRatio="766" firstSheet="1" activeTab="10" xr2:uid="{A6D689E8-9444-4F2C-A237-DAB84596CE57}"/>
+    <workbookView xWindow="16920" yWindow="2676" windowWidth="41268" windowHeight="21480" tabRatio="766" firstSheet="1" activeTab="4" xr2:uid="{A6D689E8-9444-4F2C-A237-DAB84596CE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Bootstrap Mock Generator" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="LocationLabels">Locations!$B$7:$B$22</definedName>
     <definedName name="LocationNames">Locations!$A$7:$A$22</definedName>
     <definedName name="NumBlocksLargeSurgical">'Cut-up Variables'!$G$12:$J$12</definedName>
     <definedName name="NumBlocksMega">'Cut-up Variables'!$G$11:$J$11</definedName>
@@ -53,7 +54,7 @@
     <definedName name="ProbPriorityNonCancer">'Reception Variables'!$C$6</definedName>
     <definedName name="ProbUrgentCancer">'Reception Variables'!$B$5</definedName>
     <definedName name="ProbUrgentNonCancer">'Reception Variables'!$B$6</definedName>
-    <definedName name="RunnerTimes">Locations!$B$6:$R$22</definedName>
+    <definedName name="RunnerTimes">Locations!$C$7:$R$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2992,7 +2993,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -7998,8 +7999,8 @@
   </sheetPr>
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Change default options in config.xlsx
</commit_message>
<xml_diff>
--- a/static/examples/config.xlsx
+++ b/static/examples/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\yinchi\digital-hospitals\frontend\static\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B5D908-1806-4013-A41B-4B1C456F3835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E464264-41D3-47AD-82D5-2EE637C9B05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="2676" windowWidth="41268" windowHeight="21480" tabRatio="766" firstSheet="1" activeTab="4" xr2:uid="{A6D689E8-9444-4F2C-A237-DAB84596CE57}"/>
+    <workbookView xWindow="16920" yWindow="2676" windowWidth="41268" windowHeight="21480" tabRatio="766" xr2:uid="{A6D689E8-9444-4F2C-A237-DAB84596CE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <definedName name="NumSlidesMegas">'Microtomy Variables'!$F$8:$I$8</definedName>
     <definedName name="NumSlidesSerials">'Microtomy Variables'!$F$6:$I$6</definedName>
     <definedName name="OptSpecimenBootstrap">Main!$D$2</definedName>
+    <definedName name="OptTravelTimes">Main!$D$3</definedName>
     <definedName name="ProbBMSCutup">'Cut-up Variables'!$B$6</definedName>
     <definedName name="ProbBMSCutupUrgent">'Cut-up Variables'!$C$6</definedName>
     <definedName name="ProbDecalcBone">'Processing Variables'!$B$5</definedName>
@@ -2658,8 +2659,8 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2699,7 +2700,7 @@
         <v>291</v>
       </c>
       <c r="D3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E3" t="s">
         <v>293</v>
@@ -7999,8 +8000,8 @@
   </sheetPr>
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>